<commit_message>
add braindata; debug pca
</commit_message>
<xml_diff>
--- a/main/case_studies/output/summary.xlsx
+++ b/main/case_studies/output/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/April30/benchmark-hdf5-clustering/main/case_studies/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC97BFB-F86C-DC4C-BBB1-5762A4FED12E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7C03A4-9E0E-B341-A8D4-DA04ECC9EFF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{A8B462C3-9E21-2A43-B38F-397BFBDF88BF}"/>
+    <workbookView xWindow="420" yWindow="1020" windowWidth="25440" windowHeight="15000" xr2:uid="{A8B462C3-9E21-2A43-B38F-397BFBDF88BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
   <si>
     <t>TENX_PBMC68K</t>
   </si>
   <si>
-    <t>Cells: 67991</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Batch</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>User_time</t>
   </si>
   <si>
@@ -63,20 +57,80 @@
     <t>No. of Cores</t>
   </si>
   <si>
-    <t>Genes: 6505</t>
-  </si>
-  <si>
     <t>01_full cluster</t>
   </si>
   <si>
     <t>hdf5</t>
+  </si>
+  <si>
+    <t>kmeans</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>HCA_BONEMARROW</t>
+  </si>
+  <si>
+    <t>HCA_CORDBLOOD</t>
+  </si>
+  <si>
+    <t>Cells: 329,153</t>
+  </si>
+  <si>
+    <t>Cells: 67,991</t>
+  </si>
+  <si>
+    <t>Genes: 6,505</t>
+  </si>
+  <si>
+    <t>Cells: 333,253</t>
+  </si>
+  <si>
+    <t>Genes: 7,160</t>
+  </si>
+  <si>
+    <t>Genes: 5,861</t>
+  </si>
+  <si>
+    <t>02_normalization</t>
+  </si>
+  <si>
+    <t>02_saving the normalized sce</t>
+  </si>
+  <si>
+    <t>03_realize logcounts</t>
+  </si>
+  <si>
+    <t>03_find var</t>
+  </si>
+  <si>
+    <t>B_time</t>
+  </si>
+  <si>
+    <t>** kmeans couldn't run on full data (error in do_one(nmeth) : long vectors (argument 1) are not supported in .Fortran)</t>
+  </si>
+  <si>
+    <t>** kmeans couldn't run run on full data  (error in do_one(nmeth) : long vectors (argument 1) are not supported in .Fortran)</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>B_memory</t>
+  </si>
+  <si>
+    <t>WCSS</t>
+  </si>
+  <si>
+    <t>B_wcss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,34 +139,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -120,15 +189,156 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,110 +653,586 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DCF6C0-2344-E749-A87D-9B7506BF23A1}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>82.35</v>
+      </c>
+      <c r="F5" s="10">
+        <v>7.91</v>
+      </c>
+      <c r="G5" s="10">
+        <v>91.05</v>
+      </c>
+      <c r="H5" s="15">
+        <v>2</v>
+      </c>
+      <c r="I5" s="19">
+        <v>2908.5925779999998</v>
+      </c>
+      <c r="J5" s="15">
+        <v>1</v>
+      </c>
+      <c r="K5" s="19">
+        <v>170097214.69999999</v>
+      </c>
+      <c r="L5" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>113.29</v>
+      </c>
+      <c r="F6" s="10">
+        <v>7.91</v>
+      </c>
+      <c r="G6" s="10">
+        <v>126.06</v>
+      </c>
+      <c r="H6" s="15">
+        <v>2</v>
+      </c>
+      <c r="I6" s="19">
+        <v>2890.8102220000001</v>
+      </c>
+      <c r="J6" s="15">
+        <v>1</v>
+      </c>
+      <c r="K6" s="19">
+        <v>139915933.59999999</v>
+      </c>
+      <c r="L6" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1331.5419999999999</v>
+      </c>
+      <c r="F7" s="10">
+        <v>14.515499999999999</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1346.1089999999999</v>
+      </c>
+      <c r="H7" s="15">
+        <v>2</v>
+      </c>
+      <c r="I7" s="19">
+        <v>15580.241180000001</v>
+      </c>
+      <c r="J7" s="15">
+        <v>1</v>
+      </c>
+      <c r="K7" s="19">
+        <v>132008673.40000001</v>
+      </c>
+      <c r="L7" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.92149999999999999</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.77049999999999996</v>
+      </c>
+      <c r="G8" s="10">
+        <v>577.97699999999998</v>
+      </c>
+      <c r="H8" s="15">
+        <v>2</v>
+      </c>
+      <c r="I8" s="19">
+        <v>479.6820697</v>
+      </c>
+      <c r="J8" s="15">
+        <v>1</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1.012</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G9" s="10">
+        <v>294.69099999999997</v>
+      </c>
+      <c r="H9" s="15">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14">
+        <v>109.9205</v>
+      </c>
+      <c r="F10" s="10">
+        <v>6.0605000000000002</v>
+      </c>
+      <c r="G10" s="10">
+        <v>116.26300000000001</v>
+      </c>
+      <c r="H10" s="15">
+        <v>2</v>
+      </c>
+      <c r="I10" s="19">
+        <v>835.36475689999997</v>
+      </c>
+      <c r="J10" s="15">
+        <v>2</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16">
+        <v>76.691000000000003</v>
+      </c>
+      <c r="F11" s="4">
+        <v>3.1724999999999999</v>
+      </c>
+      <c r="G11" s="4">
+        <v>79.865499999999997</v>
+      </c>
+      <c r="H11" s="17">
+        <v>1</v>
+      </c>
+      <c r="I11" s="20">
+        <v>781.99876700000004</v>
+      </c>
+      <c r="J11" s="17">
+        <v>2</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="E16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C17" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>82.35</v>
-      </c>
-      <c r="G3" s="3">
-        <v>7.91</v>
-      </c>
-      <c r="H3" s="3">
-        <v>91.05</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="14">
+        <v>433.53500000000003</v>
+      </c>
+      <c r="F17" s="10">
+        <v>42.2</v>
+      </c>
+      <c r="G17" s="10">
+        <v>479.00299999999999</v>
+      </c>
+      <c r="H17" s="15">
+        <v>1</v>
+      </c>
+      <c r="I17" s="19">
+        <v>13793.85464</v>
+      </c>
+      <c r="J17" s="15">
+        <v>1</v>
+      </c>
+      <c r="K17" s="19">
+        <v>66537663521</v>
+      </c>
+      <c r="L17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2">
         <v>0.01</v>
       </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>113.29</v>
-      </c>
-      <c r="G4" s="3">
-        <v>7.91</v>
-      </c>
-      <c r="H4" s="3">
-        <v>126.06</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>676.68</v>
+      </c>
+      <c r="F18" s="4">
+        <v>66.998000000000005</v>
+      </c>
+      <c r="G18" s="4">
+        <v>771.93700000000001</v>
+      </c>
+      <c r="H18" s="17">
+        <v>1</v>
+      </c>
+      <c r="I18" s="20">
+        <v>13817.140649999999</v>
+      </c>
+      <c r="J18" s="17">
+        <v>1</v>
+      </c>
+      <c r="K18" s="20">
+        <v>54187136853</v>
+      </c>
+      <c r="L18" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="14">
+        <v>299.97699999999998</v>
+      </c>
+      <c r="F26" s="10">
+        <v>28.751999999999999</v>
+      </c>
+      <c r="G26" s="10">
+        <v>331.03500000000003</v>
+      </c>
+      <c r="H26" s="15">
+        <v>1</v>
+      </c>
+      <c r="I26" s="19">
+        <v>11298.18924</v>
+      </c>
+      <c r="J26" s="21">
+        <v>1</v>
+      </c>
+      <c r="K26" s="19">
+        <v>24091415050</v>
+      </c>
+      <c r="L26" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="16">
+        <v>474.28500000000003</v>
+      </c>
+      <c r="F27" s="4">
+        <v>46.31</v>
+      </c>
+      <c r="G27" s="4">
+        <v>543.66499999999996</v>
+      </c>
+      <c r="H27" s="17">
+        <v>1</v>
+      </c>
+      <c r="I27" s="20">
+        <v>11298.18924</v>
+      </c>
+      <c r="J27" s="22">
+        <v>1</v>
+      </c>
+      <c r="K27" s="20">
+        <v>15415563158</v>
+      </c>
+      <c r="L27" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
seperate find most vars and pca; prepare for hca pca
</commit_message>
<xml_diff>
--- a/main/case_studies/output/summary.xlsx
+++ b/main/case_studies/output/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/April30/benchmark-hdf5-clustering/main/case_studies/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7C03A4-9E0E-B341-A8D4-DA04ECC9EFF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57FCB6C-10E3-9B4A-BC7C-86E62FC23F78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1020" windowWidth="25440" windowHeight="15000" xr2:uid="{A8B462C3-9E21-2A43-B38F-397BFBDF88BF}"/>
+    <workbookView xWindow="40960" yWindow="1200" windowWidth="31820" windowHeight="18600" xr2:uid="{A8B462C3-9E21-2A43-B38F-397BFBDF88BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>TENX_PBMC68K</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>B_wcss</t>
+  </si>
+  <si>
+    <t>03_pca</t>
   </si>
 </sst>
 </file>
@@ -653,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DCF6C0-2344-E749-A87D-9B7506BF23A1}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,7 +934,7 @@
       <c r="L10" s="15"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -943,116 +946,112 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="14">
         <v>76.691000000000003</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="10">
         <v>3.1724999999999999</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="10">
         <v>79.865499999999997</v>
       </c>
-      <c r="H11" s="17">
-        <v>1</v>
-      </c>
-      <c r="I11" s="20">
+      <c r="H11" s="15">
+        <v>1</v>
+      </c>
+      <c r="I11" s="19">
         <v>781.99876700000004</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="15">
         <v>2</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" s="16">
+        <v>1595.7059999999999</v>
+      </c>
+      <c r="F12" s="4">
+        <v>268.91899999999998</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4079.1979999999999</v>
+      </c>
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
+      <c r="I12" s="20">
+        <v>798.97522300000003</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="18" t="s">
+      <c r="L17" s="18" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" s="14">
-        <v>433.53500000000003</v>
-      </c>
-      <c r="F17" s="10">
-        <v>42.2</v>
-      </c>
-      <c r="G17" s="10">
-        <v>479.00299999999999</v>
-      </c>
-      <c r="H17" s="15">
-        <v>1</v>
-      </c>
-      <c r="I17" s="19">
-        <v>13793.85464</v>
-      </c>
-      <c r="J17" s="15">
-        <v>1</v>
-      </c>
-      <c r="K17" s="19">
-        <v>66537663521</v>
-      </c>
-      <c r="L17" s="15">
-        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1063,133 +1062,133 @@
         <v>9</v>
       </c>
       <c r="C18" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14">
+        <v>433.53500000000003</v>
+      </c>
+      <c r="F18" s="10">
+        <v>42.2</v>
+      </c>
+      <c r="G18" s="10">
+        <v>479.00299999999999</v>
+      </c>
+      <c r="H18" s="15">
+        <v>1</v>
+      </c>
+      <c r="I18" s="19">
+        <v>13793.85464</v>
+      </c>
+      <c r="J18" s="15">
+        <v>1</v>
+      </c>
+      <c r="K18" s="19">
+        <v>66537663521</v>
+      </c>
+      <c r="L18" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2">
         <v>0.01</v>
       </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="16">
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16">
         <v>676.68</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F19" s="4">
         <v>66.998000000000005</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G19" s="4">
         <v>771.93700000000001</v>
       </c>
-      <c r="H18" s="17">
-        <v>1</v>
-      </c>
-      <c r="I18" s="20">
+      <c r="H19" s="17">
+        <v>1</v>
+      </c>
+      <c r="I19" s="20">
         <v>13817.140649999999</v>
       </c>
-      <c r="J18" s="17">
-        <v>1</v>
-      </c>
-      <c r="K18" s="20">
+      <c r="J19" s="17">
+        <v>1</v>
+      </c>
+      <c r="K19" s="20">
         <v>54187136853</v>
       </c>
-      <c r="L18" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="L19" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F26" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G26" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H26" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I26" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J25" s="18" t="s">
+      <c r="J26" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K26" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L25" s="18" t="s">
+      <c r="L26" s="18" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1</v>
-      </c>
-      <c r="E26" s="14">
-        <v>299.97699999999998</v>
-      </c>
-      <c r="F26" s="10">
-        <v>28.751999999999999</v>
-      </c>
-      <c r="G26" s="10">
-        <v>331.03500000000003</v>
-      </c>
-      <c r="H26" s="15">
-        <v>1</v>
-      </c>
-      <c r="I26" s="19">
-        <v>11298.18924</v>
-      </c>
-      <c r="J26" s="21">
-        <v>1</v>
-      </c>
-      <c r="K26" s="19">
-        <v>24091415050</v>
-      </c>
-      <c r="L26" s="15">
-        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1200,38 +1199,76 @@
         <v>9</v>
       </c>
       <c r="C27" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="14">
+        <v>299.97699999999998</v>
+      </c>
+      <c r="F27" s="10">
+        <v>28.751999999999999</v>
+      </c>
+      <c r="G27" s="10">
+        <v>331.03500000000003</v>
+      </c>
+      <c r="H27" s="15">
+        <v>1</v>
+      </c>
+      <c r="I27" s="19">
+        <v>11298.18924</v>
+      </c>
+      <c r="J27" s="21">
+        <v>1</v>
+      </c>
+      <c r="K27" s="19">
+        <v>24091415050</v>
+      </c>
+      <c r="L27" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2">
         <v>0.01</v>
       </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="16">
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="16">
         <v>474.28500000000003</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F28" s="4">
         <v>46.31</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G28" s="4">
         <v>543.66499999999996</v>
       </c>
-      <c r="H27" s="17">
-        <v>1</v>
-      </c>
-      <c r="I27" s="20">
+      <c r="H28" s="17">
+        <v>1</v>
+      </c>
+      <c r="I28" s="20">
         <v>11298.18924</v>
       </c>
-      <c r="J27" s="22">
-        <v>1</v>
-      </c>
-      <c r="K27" s="20">
+      <c r="J28" s="22">
+        <v>1</v>
+      </c>
+      <c r="K28" s="20">
         <v>15415563158</v>
       </c>
-      <c r="L27" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="L28" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>